<commit_message>
Se agrego la funcion unir_datos
</commit_message>
<xml_diff>
--- a/prueba.xlsx
+++ b/prueba.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,55 +436,71 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>objeto</t>
+          <t>Tiempo</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>tiempo</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>distancia</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>acceleration</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>velocidad</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>objeto_distancia</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>uno</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
+        <v>-20</v>
+      </c>
+      <c r="D2" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>-10</v>
+      </c>
+      <c r="D3" t="n">
         <v>20</v>
       </c>
-      <c r="D2" t="n">
-        <v>32</v>
-      </c>
-      <c r="E2" t="n">
-        <v>39</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="n">
+        <v>-6.666666666666667</v>
+      </c>
+      <c r="D4" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>-5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>